<commit_message>
Started ROK and Japan Ship Analysis
</commit_message>
<xml_diff>
--- a/Output/Shipbuilding/DOD_Shipbuilding_Contracts.xlsx
+++ b/Output/Shipbuilding/DOD_Shipbuilding_Contracts.xlsx
@@ -239,12 +239,12 @@
   <numFmts count="8">
     <numFmt numFmtId="172" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="192" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="212" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="217" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="214" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="196" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="215" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="211" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="216" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="218" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="219" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -285,12 +285,12 @@
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="172" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="192" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="212" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="217" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="214" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="196" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="215" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="211" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="216" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="218" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="219" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>